<commit_message>
fix n style: fix view n style base file
</commit_message>
<xml_diff>
--- a/storage/app/public/assets/excel/template.xlsx
+++ b/storage/app/public/assets/excel/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\final-assignment\performance-achievement-information-system-of-FTI-ITERA\storage\app\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{817EA50F-3174-45F9-8CA6-207BC33C0447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E44FF5-B674-4ACE-95FE-AA9CC31766D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -58,9 +58,6 @@
     <t>Indikator Kinerja</t>
   </si>
   <si>
-    <t>Tipe (persen, angka, persen)</t>
-  </si>
-  <si>
     <t>ss1</t>
   </si>
   <si>
@@ -137,6 +134,9 @@
   </si>
   <si>
     <t>3. Cell A2 tidak boleh kosong</t>
+  </si>
+  <si>
+    <t>Tipe (teks, angka, persen)</t>
   </si>
 </sst>
 </file>
@@ -518,8 +518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +539,7 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -552,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEA56A4-A36A-48BA-84D7-28E0D05906D8}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,15 +575,15 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -595,7 +595,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -608,7 +608,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -621,16 +621,16 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>3</v>
@@ -641,69 +641,69 @@
       <c r="A6" s="3"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="8" t="s">
         <v>2</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>20</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>6</v>
@@ -711,27 +711,27 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>